<commit_message>
added demos to the readme
</commit_message>
<xml_diff>
--- a/data/example_db.xlsx
+++ b/data/example_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenekim/ml-projects/sql_llm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenekim/ml-projects/sql_llm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A52856-2B42-7945-A390-88D140E8CCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B7B9EF-A22D-C948-AF30-219F1F65A7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref_table" sheetId="1" r:id="rId1"/>
@@ -541,11 +541,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -743,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB372A2B-3566-7149-B44E-989C8E8A82BF}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>